<commit_message>
Fix race conditions for entity data rollback
Needed to change the entity save process, so refactored some tests and
entity views. Modified test input data files to have a unique id for
each row so that they will work with tests.
</commit_message>
<xml_diff>
--- a/misc/test_files/entity_data_6_large.xlsx
+++ b/misc/test_files/entity_data_6_large.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="214">
   <si>
     <t xml:space="preserve">transaction_quantity</t>
   </si>
@@ -44,6 +44,624 @@
   </si>
   <si>
     <t xml:space="preserve">293-64-2300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7621</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2301</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7622</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2302</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7623</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2303</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7624</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2304</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7625</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2305</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7626</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2306</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7627</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2307</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7628</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2308</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7629</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2309</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7630</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2310</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7631</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2311</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7632</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2312</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7633</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2313</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7634</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2314</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7635</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2315</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7636</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2316</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7637</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2317</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7638</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2318</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7639</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2319</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7640</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2320</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7641</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7642</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2322</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7643</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7644</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2324</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7645</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2325</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7646</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2326</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7647</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2327</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7648</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2328</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7649</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2329</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7650</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2330</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7651</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2331</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7652</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2332</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7653</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2333</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7654</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2334</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7655</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2335</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7656</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2336</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7657</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2337</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7658</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2338</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7659</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2339</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7660</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2340</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7661</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2341</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7662</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2342</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7663</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2343</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7664</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2344</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7665</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7666</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2346</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7667</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2347</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7668</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2348</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7669</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2349</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7670</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2350</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7671</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2351</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7672</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2352</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7673</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2353</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7674</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2354</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7675</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2355</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7676</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2356</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7677</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2357</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7678</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2358</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7679</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2359</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7680</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2360</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7681</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2361</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7682</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2362</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7683</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2363</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7684</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2364</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7685</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2365</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7686</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2366</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7687</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2367</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7688</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2368</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7689</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2369</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7690</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2370</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7691</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2371</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7692</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2372</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7693</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2373</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7694</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2374</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7695</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2375</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7696</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2376</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7697</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2377</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7698</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2378</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7699</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2379</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2380</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7701</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2381</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7702</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2382</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7703</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2383</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7704</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2384</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7705</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2385</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7706</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2386</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7707</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2387</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7708</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2388</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7709</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2389</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7710</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2390</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7711</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2391</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7712</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2392</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7713</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2393</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7714</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2394</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7715</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2395</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7716</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2396</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7717</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2397</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7718</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2398</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7719</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2399</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7720</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7721</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2401</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7722</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">988-90-7723</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293-64-2403</t>
   </si>
 </sst>
 </file>
@@ -58,6 +676,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -141,18 +760,18 @@
   </sheetPr>
   <dimension ref="A1:E105"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E104" activeCellId="0" sqref="E104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2704081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1377551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.015306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9744897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3010204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3775510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.3367346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="14.5816326530612"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -197,10 +816,10 @@
         <v>5</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>320.89</v>
@@ -214,10 +833,10 @@
         <v>5</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>320.89</v>
@@ -231,10 +850,10 @@
         <v>5</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>320.89</v>
@@ -248,10 +867,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>320.89</v>
@@ -265,10 +884,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>320.89</v>
@@ -282,10 +901,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>320.89</v>
@@ -299,10 +918,10 @@
         <v>5</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>320.89</v>
@@ -316,10 +935,10 @@
         <v>5</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>320.89</v>
@@ -333,10 +952,10 @@
         <v>5</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>320.89</v>
@@ -350,10 +969,10 @@
         <v>5</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>320.89</v>
@@ -367,10 +986,10 @@
         <v>5</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>320.89</v>
@@ -384,10 +1003,10 @@
         <v>5</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>320.89</v>
@@ -401,10 +1020,10 @@
         <v>5</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>320.89</v>
@@ -418,10 +1037,10 @@
         <v>5</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>320.89</v>
@@ -435,10 +1054,10 @@
         <v>5</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>320.89</v>
@@ -452,10 +1071,10 @@
         <v>5</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>320.89</v>
@@ -469,10 +1088,10 @@
         <v>5</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>320.89</v>
@@ -486,10 +1105,10 @@
         <v>5</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>320.89</v>
@@ -503,10 +1122,10 @@
         <v>5</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>320.89</v>
@@ -520,10 +1139,10 @@
         <v>5</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="E22" s="0" t="n">
         <v>320.89</v>
@@ -537,10 +1156,10 @@
         <v>5</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>320.89</v>
@@ -554,10 +1173,10 @@
         <v>5</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>320.89</v>
@@ -571,10 +1190,10 @@
         <v>5</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>320.89</v>
@@ -588,10 +1207,10 @@
         <v>5</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>320.89</v>
@@ -605,10 +1224,10 @@
         <v>5</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>320.89</v>
@@ -622,10 +1241,10 @@
         <v>5</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
       <c r="E28" s="0" t="n">
         <v>320.89</v>
@@ -639,10 +1258,10 @@
         <v>5</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>320.89</v>
@@ -656,10 +1275,10 @@
         <v>5</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>320.89</v>
@@ -673,10 +1292,10 @@
         <v>5</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="E31" s="0" t="n">
         <v>320.89</v>
@@ -690,10 +1309,10 @@
         <v>5</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="E32" s="0" t="n">
         <v>320.89</v>
@@ -707,10 +1326,10 @@
         <v>5</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="E33" s="0" t="n">
         <v>320.89</v>
@@ -724,10 +1343,10 @@
         <v>5</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>6</v>
+        <v>70</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="E34" s="0" t="n">
         <v>320.89</v>
@@ -741,10 +1360,10 @@
         <v>5</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>6</v>
+        <v>72</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="E35" s="0" t="n">
         <v>320.89</v>
@@ -758,10 +1377,10 @@
         <v>5</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>6</v>
+        <v>74</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="E36" s="0" t="n">
         <v>320.89</v>
@@ -775,10 +1394,10 @@
         <v>5</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>6</v>
+        <v>76</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="E37" s="0" t="n">
         <v>320.89</v>
@@ -792,10 +1411,10 @@
         <v>5</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>6</v>
+        <v>78</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>7</v>
+        <v>79</v>
       </c>
       <c r="E38" s="0" t="n">
         <v>320.89</v>
@@ -809,10 +1428,10 @@
         <v>5</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>7</v>
+        <v>81</v>
       </c>
       <c r="E39" s="0" t="n">
         <v>320.89</v>
@@ -826,10 +1445,10 @@
         <v>5</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>6</v>
+        <v>82</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>7</v>
+        <v>83</v>
       </c>
       <c r="E40" s="0" t="n">
         <v>320.89</v>
@@ -843,10 +1462,10 @@
         <v>5</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>6</v>
+        <v>84</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="E41" s="0" t="n">
         <v>320.89</v>
@@ -860,10 +1479,10 @@
         <v>5</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>6</v>
+        <v>86</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>7</v>
+        <v>87</v>
       </c>
       <c r="E42" s="0" t="n">
         <v>320.89</v>
@@ -877,10 +1496,10 @@
         <v>5</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>6</v>
+        <v>88</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="E43" s="0" t="n">
         <v>320.89</v>
@@ -894,10 +1513,10 @@
         <v>5</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>6</v>
+        <v>90</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>7</v>
+        <v>91</v>
       </c>
       <c r="E44" s="0" t="n">
         <v>320.89</v>
@@ -911,10 +1530,10 @@
         <v>5</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="E45" s="0" t="n">
         <v>320.89</v>
@@ -928,10 +1547,10 @@
         <v>5</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>6</v>
+        <v>94</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>7</v>
+        <v>95</v>
       </c>
       <c r="E46" s="0" t="n">
         <v>320.89</v>
@@ -945,10 +1564,10 @@
         <v>5</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>6</v>
+        <v>96</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>7</v>
+        <v>97</v>
       </c>
       <c r="E47" s="0" t="n">
         <v>320.89</v>
@@ -962,10 +1581,10 @@
         <v>5</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>7</v>
+        <v>99</v>
       </c>
       <c r="E48" s="0" t="n">
         <v>320.89</v>
@@ -979,10 +1598,10 @@
         <v>5</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>6</v>
+        <v>100</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>7</v>
+        <v>101</v>
       </c>
       <c r="E49" s="0" t="n">
         <v>320.89</v>
@@ -996,10 +1615,10 @@
         <v>5</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>6</v>
+        <v>102</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="E50" s="0" t="n">
         <v>320.89</v>
@@ -1013,10 +1632,10 @@
         <v>5</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>6</v>
+        <v>104</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>7</v>
+        <v>105</v>
       </c>
       <c r="E51" s="0" t="n">
         <v>320.89</v>
@@ -1030,10 +1649,10 @@
         <v>5</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>6</v>
+        <v>106</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>7</v>
+        <v>107</v>
       </c>
       <c r="E52" s="0" t="n">
         <v>320.89</v>
@@ -1047,10 +1666,10 @@
         <v>5</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>6</v>
+        <v>108</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>7</v>
+        <v>109</v>
       </c>
       <c r="E53" s="0" t="n">
         <v>320.89</v>
@@ -1064,10 +1683,10 @@
         <v>5</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>6</v>
+        <v>110</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>7</v>
+        <v>111</v>
       </c>
       <c r="E54" s="0" t="n">
         <v>320.89</v>
@@ -1081,10 +1700,10 @@
         <v>5</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>6</v>
+        <v>112</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>7</v>
+        <v>113</v>
       </c>
       <c r="E55" s="0" t="n">
         <v>320.89</v>
@@ -1098,10 +1717,10 @@
         <v>5</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>6</v>
+        <v>114</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>7</v>
+        <v>115</v>
       </c>
       <c r="E56" s="0" t="n">
         <v>320.89</v>
@@ -1115,10 +1734,10 @@
         <v>5</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>6</v>
+        <v>116</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>7</v>
+        <v>117</v>
       </c>
       <c r="E57" s="0" t="n">
         <v>320.89</v>
@@ -1132,10 +1751,10 @@
         <v>5</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>6</v>
+        <v>118</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>7</v>
+        <v>119</v>
       </c>
       <c r="E58" s="0" t="n">
         <v>320.89</v>
@@ -1149,10 +1768,10 @@
         <v>5</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>6</v>
+        <v>120</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>7</v>
+        <v>121</v>
       </c>
       <c r="E59" s="0" t="n">
         <v>320.89</v>
@@ -1166,10 +1785,10 @@
         <v>5</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>6</v>
+        <v>122</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>7</v>
+        <v>123</v>
       </c>
       <c r="E60" s="0" t="n">
         <v>320.89</v>
@@ -1183,10 +1802,10 @@
         <v>5</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>6</v>
+        <v>124</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>7</v>
+        <v>125</v>
       </c>
       <c r="E61" s="0" t="n">
         <v>320.89</v>
@@ -1200,10 +1819,10 @@
         <v>5</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>6</v>
+        <v>126</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>7</v>
+        <v>127</v>
       </c>
       <c r="E62" s="0" t="n">
         <v>320.89</v>
@@ -1217,10 +1836,10 @@
         <v>5</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>6</v>
+        <v>128</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>7</v>
+        <v>129</v>
       </c>
       <c r="E63" s="0" t="n">
         <v>320.89</v>
@@ -1234,10 +1853,10 @@
         <v>5</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>6</v>
+        <v>130</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>7</v>
+        <v>131</v>
       </c>
       <c r="E64" s="0" t="n">
         <v>320.89</v>
@@ -1251,10 +1870,10 @@
         <v>5</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>6</v>
+        <v>132</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>7</v>
+        <v>133</v>
       </c>
       <c r="E65" s="0" t="n">
         <v>320.89</v>
@@ -1268,10 +1887,10 @@
         <v>5</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>6</v>
+        <v>134</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>7</v>
+        <v>135</v>
       </c>
       <c r="E66" s="0" t="n">
         <v>320.89</v>
@@ -1285,10 +1904,10 @@
         <v>5</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>6</v>
+        <v>136</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>7</v>
+        <v>137</v>
       </c>
       <c r="E67" s="0" t="n">
         <v>320.89</v>
@@ -1302,10 +1921,10 @@
         <v>5</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>6</v>
+        <v>138</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>7</v>
+        <v>139</v>
       </c>
       <c r="E68" s="0" t="n">
         <v>320.89</v>
@@ -1319,10 +1938,10 @@
         <v>5</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>7</v>
+        <v>141</v>
       </c>
       <c r="E69" s="0" t="n">
         <v>320.89</v>
@@ -1336,10 +1955,10 @@
         <v>5</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>6</v>
+        <v>142</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>7</v>
+        <v>143</v>
       </c>
       <c r="E70" s="0" t="n">
         <v>320.89</v>
@@ -1353,10 +1972,10 @@
         <v>5</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>6</v>
+        <v>144</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>7</v>
+        <v>145</v>
       </c>
       <c r="E71" s="0" t="n">
         <v>320.89</v>
@@ -1370,10 +1989,10 @@
         <v>5</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>7</v>
+        <v>147</v>
       </c>
       <c r="E72" s="0" t="n">
         <v>320.89</v>
@@ -1387,10 +2006,10 @@
         <v>5</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>6</v>
+        <v>148</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>7</v>
+        <v>149</v>
       </c>
       <c r="E73" s="0" t="n">
         <v>320.89</v>
@@ -1404,10 +2023,10 @@
         <v>5</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>6</v>
+        <v>150</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>7</v>
+        <v>151</v>
       </c>
       <c r="E74" s="0" t="n">
         <v>320.89</v>
@@ -1421,10 +2040,10 @@
         <v>5</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>6</v>
+        <v>152</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>7</v>
+        <v>153</v>
       </c>
       <c r="E75" s="0" t="n">
         <v>320.89</v>
@@ -1438,10 +2057,10 @@
         <v>5</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>6</v>
+        <v>154</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>7</v>
+        <v>155</v>
       </c>
       <c r="E76" s="0" t="n">
         <v>320.89</v>
@@ -1455,10 +2074,10 @@
         <v>5</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>6</v>
+        <v>156</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>7</v>
+        <v>157</v>
       </c>
       <c r="E77" s="0" t="n">
         <v>320.89</v>
@@ -1472,10 +2091,10 @@
         <v>5</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>6</v>
+        <v>158</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>7</v>
+        <v>159</v>
       </c>
       <c r="E78" s="0" t="n">
         <v>320.89</v>
@@ -1489,10 +2108,10 @@
         <v>5</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>6</v>
+        <v>160</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>7</v>
+        <v>161</v>
       </c>
       <c r="E79" s="0" t="n">
         <v>320.89</v>
@@ -1506,10 +2125,10 @@
         <v>5</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>6</v>
+        <v>162</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>7</v>
+        <v>163</v>
       </c>
       <c r="E80" s="0" t="n">
         <v>320.89</v>
@@ -1523,10 +2142,10 @@
         <v>5</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>6</v>
+        <v>164</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>7</v>
+        <v>165</v>
       </c>
       <c r="E81" s="0" t="n">
         <v>320.89</v>
@@ -1540,10 +2159,10 @@
         <v>5</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>6</v>
+        <v>166</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>7</v>
+        <v>167</v>
       </c>
       <c r="E82" s="0" t="n">
         <v>320.89</v>
@@ -1557,10 +2176,10 @@
         <v>5</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>6</v>
+        <v>168</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>7</v>
+        <v>169</v>
       </c>
       <c r="E83" s="0" t="n">
         <v>320.89</v>
@@ -1574,10 +2193,10 @@
         <v>5</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>6</v>
+        <v>170</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>7</v>
+        <v>171</v>
       </c>
       <c r="E84" s="0" t="n">
         <v>320.89</v>
@@ -1591,10 +2210,10 @@
         <v>5</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>6</v>
+        <v>172</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>7</v>
+        <v>173</v>
       </c>
       <c r="E85" s="0" t="n">
         <v>320.89</v>
@@ -1608,10 +2227,10 @@
         <v>5</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>6</v>
+        <v>174</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>7</v>
+        <v>175</v>
       </c>
       <c r="E86" s="0" t="n">
         <v>320.89</v>
@@ -1625,10 +2244,10 @@
         <v>5</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>6</v>
+        <v>176</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>7</v>
+        <v>177</v>
       </c>
       <c r="E87" s="0" t="n">
         <v>320.89</v>
@@ -1642,10 +2261,10 @@
         <v>5</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>6</v>
+        <v>178</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>7</v>
+        <v>179</v>
       </c>
       <c r="E88" s="0" t="n">
         <v>320.89</v>
@@ -1659,10 +2278,10 @@
         <v>5</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>6</v>
+        <v>180</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>7</v>
+        <v>181</v>
       </c>
       <c r="E89" s="0" t="n">
         <v>320.89</v>
@@ -1676,10 +2295,10 @@
         <v>5</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>6</v>
+        <v>182</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>7</v>
+        <v>183</v>
       </c>
       <c r="E90" s="0" t="n">
         <v>320.89</v>
@@ -1693,10 +2312,10 @@
         <v>5</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>6</v>
+        <v>184</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>7</v>
+        <v>185</v>
       </c>
       <c r="E91" s="0" t="n">
         <v>320.89</v>
@@ -1710,10 +2329,10 @@
         <v>5</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>6</v>
+        <v>186</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>7</v>
+        <v>187</v>
       </c>
       <c r="E92" s="0" t="n">
         <v>320.89</v>
@@ -1727,10 +2346,10 @@
         <v>5</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>6</v>
+        <v>188</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>7</v>
+        <v>189</v>
       </c>
       <c r="E93" s="0" t="n">
         <v>320.89</v>
@@ -1744,10 +2363,10 @@
         <v>5</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>6</v>
+        <v>190</v>
       </c>
       <c r="D94" s="0" t="s">
-        <v>7</v>
+        <v>191</v>
       </c>
       <c r="E94" s="0" t="n">
         <v>320.89</v>
@@ -1761,10 +2380,10 @@
         <v>5</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>6</v>
+        <v>192</v>
       </c>
       <c r="D95" s="0" t="s">
-        <v>7</v>
+        <v>193</v>
       </c>
       <c r="E95" s="0" t="n">
         <v>320.89</v>
@@ -1778,10 +2397,10 @@
         <v>5</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>6</v>
+        <v>194</v>
       </c>
       <c r="D96" s="0" t="s">
-        <v>7</v>
+        <v>195</v>
       </c>
       <c r="E96" s="0" t="n">
         <v>320.89</v>
@@ -1795,10 +2414,10 @@
         <v>5</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>7</v>
+        <v>197</v>
       </c>
       <c r="E97" s="0" t="n">
         <v>320.89</v>
@@ -1812,10 +2431,10 @@
         <v>5</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>6</v>
+        <v>198</v>
       </c>
       <c r="D98" s="0" t="s">
-        <v>7</v>
+        <v>199</v>
       </c>
       <c r="E98" s="0" t="n">
         <v>320.89</v>
@@ -1829,10 +2448,10 @@
         <v>5</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>6</v>
+        <v>200</v>
       </c>
       <c r="D99" s="0" t="s">
-        <v>7</v>
+        <v>201</v>
       </c>
       <c r="E99" s="0" t="n">
         <v>320.89</v>
@@ -1846,10 +2465,10 @@
         <v>5</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>6</v>
+        <v>202</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>7</v>
+        <v>203</v>
       </c>
       <c r="E100" s="0" t="n">
         <v>320.89</v>
@@ -1863,10 +2482,10 @@
         <v>5</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>6</v>
+        <v>204</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>7</v>
+        <v>205</v>
       </c>
       <c r="E101" s="0" t="n">
         <v>320.89</v>
@@ -1880,10 +2499,10 @@
         <v>5</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>6</v>
+        <v>206</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>7</v>
+        <v>207</v>
       </c>
       <c r="E102" s="0" t="n">
         <v>320.89</v>
@@ -1897,10 +2516,10 @@
         <v>5</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>6</v>
+        <v>208</v>
       </c>
       <c r="D103" s="0" t="s">
-        <v>7</v>
+        <v>209</v>
       </c>
       <c r="E103" s="0" t="n">
         <v>320.89</v>
@@ -1914,10 +2533,10 @@
         <v>5</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>6</v>
+        <v>210</v>
       </c>
       <c r="D104" s="0" t="s">
-        <v>7</v>
+        <v>211</v>
       </c>
       <c r="E104" s="0" t="n">
         <v>320.89</v>
@@ -1931,10 +2550,10 @@
         <v>5</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>6</v>
+        <v>212</v>
       </c>
       <c r="D105" s="0" t="s">
-        <v>7</v>
+        <v>213</v>
       </c>
       <c r="E105" s="0" t="n">
         <v>320.89</v>

</xml_diff>